<commit_message>
feat: Enhance Bank Statement Import functionality with auto-generation of statement number, date, and closing balance; add demo import API script
</commit_message>
<xml_diff>
--- a/bank_statement_sample.xlsx
+++ b/bank_statement_sample.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,207 +514,183 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-15</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-15</t>
-        </is>
-      </c>
+      <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr"/>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>CREDIT</t>
+          <t>Opening Balance</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr"/>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>5000.00</t>
-        </is>
-      </c>
+      <c r="F2" s="2" t="inlineStr"/>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>25000.00</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>SAL-2026-01</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>Salary Deposit</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Employer Inc</t>
-        </is>
-      </c>
+          <t>20000.00</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr"/>
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>DEBIT</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>1200.00</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr"/>
+          <t>CREDIT</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>5000.00</t>
+        </is>
+      </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>23800.00</t>
+          <t>25000.00</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>CHQ-001</t>
+          <t>SAL-2026-01</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>Rent Payment</t>
+          <t>Salary Deposit</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>ABC Properties</t>
+          <t>Employer Inc</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>CREDIT</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>350.00</t>
-        </is>
-      </c>
+          <t>DEBIT</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>1200.00</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr"/>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>24150.00</t>
+          <t>23800.00</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>TRF-456</t>
+          <t>CHQ-001</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>Refund from Vendor</t>
+          <t>Rent Payment</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>XYZ Supplies</t>
+          <t>ABC Properties</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>DEBIT</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>75.50</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr"/>
+          <t>CREDIT</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>350.00</t>
+        </is>
+      </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>24074.50</t>
+          <t>24150.00</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>ATM-789</t>
+          <t>TRF-456</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>ATM Withdrawal</t>
-        </is>
-      </c>
-      <c r="J5" s="2" t="inlineStr"/>
+          <t>Refund from Vendor</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>XYZ Supplies</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -724,170 +700,214 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>450.00</t>
+          <t>75.50</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr"/>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>23624.50</t>
+          <t>24074.50</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>INV-1001</t>
+          <t>ATM-789</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>Office Supplies Purchase</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>Office Depot</t>
-        </is>
-      </c>
+          <t>ATM Withdrawal</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>CREDIT</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr"/>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>2500.00</t>
-        </is>
-      </c>
+          <t>DEBIT</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>450.00</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr"/>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>26124.50</t>
+          <t>23624.50</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>DEP-123</t>
+          <t>INV-1001</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>Customer Payment</t>
+          <t>Office Supplies Purchase</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>Acme Corp</t>
+          <t>Office Depot</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>DEBIT</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>1500.00</t>
-        </is>
-      </c>
-      <c r="F8" s="2" t="inlineStr"/>
+          <t>CREDIT</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr"/>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>2500.00</t>
+        </is>
+      </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>24624.50</t>
+          <t>26124.50</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>CHQ-002</t>
+          <t>DEP-123</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>Utility Bill Payment</t>
+          <t>Customer Payment</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>Power Company</t>
+          <t>Acme Corp</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-28</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>DEBIT</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>1500.00</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr"/>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>24624.50</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>CHQ-002</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>Utility Bill Payment</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>Power Company</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
           <t>8</t>
         </is>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>2026-01-30</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C10" s="2" t="inlineStr">
         <is>
           <t>2026-01-30</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D10" s="2" t="inlineStr">
         <is>
           <t>CREDIT</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr"/>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="E10" s="2" t="inlineStr"/>
+      <c r="F10" s="2" t="inlineStr">
         <is>
           <t>800.00</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+      <c r="G10" s="2" t="inlineStr">
         <is>
           <t>25424.50</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="H10" s="2" t="inlineStr">
         <is>
           <t>TRF-789</t>
         </is>
       </c>
-      <c r="I9" s="2" t="inlineStr">
+      <c r="I10" s="2" t="inlineStr">
         <is>
           <t>Interest Credit</t>
         </is>
       </c>
-      <c r="J9" s="2" t="inlineStr">
+      <c r="J10" s="2" t="inlineStr">
         <is>
           <t>ABC Bank</t>
         </is>

</xml_diff>